<commit_message>
update with bigger range of total requests
</commit_message>
<xml_diff>
--- a/utils/pricing_estimate.xlsx
+++ b/utils/pricing_estimate.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prbejgum\Documents\azure\practice\glasswall_solutions\p-k8-jmeter-test-engine-v1\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C817B6C-1A0F-4E9C-94CF-913498D4F5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1834ED6A-E661-4F96-A5C5-80946FD288E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4960AB14-B5A5-4162-B250-4B87383966BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4960AB14-B5A5-4162-B250-4B87383966BE}"/>
   </bookViews>
   <sheets>
-    <sheet name="v1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t>Total Users</t>
-  </si>
-  <si>
-    <t>Users per pod</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>No. of nodes required</t>
   </si>
@@ -50,9 +45,6 @@
     <t>B4MS</t>
   </si>
   <si>
-    <t>Total nodes price</t>
-  </si>
-  <si>
     <t>Pod memory in MB</t>
   </si>
   <si>
@@ -83,28 +75,10 @@
     <t>F16s</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Usage: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Populate rows from 2 to 10 and based on the inputs provided, values in rows from 12 to 17 will be populated</t>
-    </r>
+    <t>Total Requests</t>
+  </si>
+  <si>
+    <t>Requests per pod</t>
   </si>
   <si>
     <r>
@@ -126,11 +100,61 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>The above Price estimation is for per hour price</t>
+      <t>The above Price estimation is for per hour price. The nodes(VMs) are billed per minute. So, for example if the tests run for 30 mins, half of the above price will be billed</t>
     </r>
   </si>
   <si>
-    <t>Max concurrent requests and total requests is equal to total users in Row 1</t>
+    <t>Total nodes price/hr</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Usage: 
+1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Populate rows from 2 to 4 based on resource requirements of the pod
+2. Populate rows from 7 to 10 based on node size used in the cluster
+3. Based on the inputs provided, values in rows from 12 to 17 will be populated. Based on values calculated in row 14 and 17, we can understand which node size is best suitable reducing the resource wastage and price</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This sheet calculates the pricing with varying number of requests for a given node size and fixed pod resources requirement.
+Use sheet1 to decide which node size is best to reduce the overall price and resource wastage.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -162,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -170,16 +194,110 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B419E4-21EB-467A-8186-C2A6A1389FC7}">
-  <dimension ref="B1:F23"/>
+  <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,7 +628,7 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3">
         <v>100000</v>
@@ -527,7 +645,7 @@
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -544,7 +662,7 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -561,7 +679,7 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>500</v>
@@ -578,24 +696,24 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -612,7 +730,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -629,7 +747,7 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>0.188</v>
@@ -646,7 +764,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <f>C8*1000/C3</f>
@@ -667,28 +785,28 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <f>C9*1024/C4</f>
-        <v>32.768000000000001</v>
+        <f>ROUNDDOWN(C9*1024/C4,0)</f>
+        <v>32</v>
       </c>
       <c r="D13">
-        <f>D9*1024/D4</f>
-        <v>98.304000000000002</v>
+        <f>ROUNDDOWN(D9*1024/D4,0)</f>
+        <v>98</v>
       </c>
       <c r="E13">
-        <f>E9*1024/E4</f>
-        <v>65.536000000000001</v>
+        <f>ROUNDDOWN(E9*1024/E4,0)</f>
+        <v>65</v>
       </c>
       <c r="F13">
-        <f>F9*1024/F4</f>
-        <v>65.536000000000001</v>
+        <f>ROUNDDOWN(F9*1024/F4,0)</f>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <f>MIN(C12,C13)</f>
@@ -709,7 +827,7 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2">
         <f>ROUNDUP(C1/C2/C14, 0)</f>
@@ -730,7 +848,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <f>C10*C16</f>
@@ -749,22 +867,471 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="2:6" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1FCD5F-5B65-453D-9623-5E98B47BA79B}">
+  <dimension ref="B1:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6">
+        <v>10</v>
+      </c>
+      <c r="D1" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E1" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F1" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G1" s="6">
+        <v>500000</v>
+      </c>
+      <c r="H1" s="6">
+        <v>800000</v>
+      </c>
+      <c r="I1" s="7">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="9">
+        <v>100</v>
+      </c>
+      <c r="D2" s="9">
+        <v>100</v>
+      </c>
+      <c r="E2" s="9">
+        <v>100</v>
+      </c>
+      <c r="F2" s="9">
+        <v>100</v>
+      </c>
+      <c r="G2" s="9">
+        <v>100</v>
+      </c>
+      <c r="H2" s="9">
+        <v>100</v>
+      </c>
+      <c r="I2" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9">
+        <v>250</v>
+      </c>
+      <c r="D3" s="9">
+        <v>250</v>
+      </c>
+      <c r="E3" s="9">
+        <v>250</v>
+      </c>
+      <c r="F3" s="9">
+        <v>250</v>
+      </c>
+      <c r="G3" s="9">
+        <v>250</v>
+      </c>
+      <c r="H3" s="9">
+        <v>250</v>
+      </c>
+      <c r="I3" s="10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9">
+        <v>500</v>
+      </c>
+      <c r="D4" s="9">
+        <v>500</v>
+      </c>
+      <c r="E4" s="9">
+        <v>500</v>
+      </c>
+      <c r="F4" s="9">
+        <v>500</v>
+      </c>
+      <c r="G4" s="9">
+        <v>500</v>
+      </c>
+      <c r="H4" s="9">
+        <v>500</v>
+      </c>
+      <c r="I4" s="10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="D7" s="9">
+        <v>16</v>
+      </c>
+      <c r="E7" s="9">
+        <v>16</v>
+      </c>
+      <c r="F7" s="9">
+        <v>16</v>
+      </c>
+      <c r="G7" s="9">
+        <v>16</v>
+      </c>
+      <c r="H7" s="9">
+        <v>16</v>
+      </c>
+      <c r="I7" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9">
+        <v>32</v>
+      </c>
+      <c r="D8" s="9">
+        <v>32</v>
+      </c>
+      <c r="E8" s="9">
+        <v>32</v>
+      </c>
+      <c r="F8" s="9">
+        <v>32</v>
+      </c>
+      <c r="G8" s="9">
+        <v>32</v>
+      </c>
+      <c r="H8" s="9">
+        <v>32</v>
+      </c>
+      <c r="I8" s="10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9">
+        <f>C7*1000/C3</f>
+        <v>64</v>
+      </c>
+      <c r="D11" s="9">
+        <f>D7*1000/D3</f>
+        <v>64</v>
+      </c>
+      <c r="E11" s="9">
+        <f>E7*1000/E3</f>
+        <v>64</v>
+      </c>
+      <c r="F11" s="9">
+        <f>F7*1000/F3</f>
+        <v>64</v>
+      </c>
+      <c r="G11" s="9">
+        <f>G7*1000/G3</f>
+        <v>64</v>
+      </c>
+      <c r="H11" s="9">
+        <f>H7*1000/H3</f>
+        <v>64</v>
+      </c>
+      <c r="I11" s="10">
+        <f>I7*1000/I3</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="9">
+        <f>ROUNDDOWN(C8*1024/C4,0)</f>
+        <v>65</v>
+      </c>
+      <c r="D12" s="9">
+        <f>ROUNDDOWN(D8*1024/D4,0)</f>
+        <v>65</v>
+      </c>
+      <c r="E12" s="9">
+        <f>ROUNDDOWN(E8*1024/E4,0)</f>
+        <v>65</v>
+      </c>
+      <c r="F12" s="9">
+        <f>ROUNDDOWN(F8*1024/F4,0)</f>
+        <v>65</v>
+      </c>
+      <c r="G12" s="9">
+        <f>ROUNDDOWN(G8*1024/G4,0)</f>
+        <v>65</v>
+      </c>
+      <c r="H12" s="9">
+        <f>ROUNDDOWN(H8*1024/H4,0)</f>
+        <v>65</v>
+      </c>
+      <c r="I12" s="10">
+        <f>ROUNDDOWN(I8*1024/I4,0)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9">
+        <f>MIN(C11,C12)</f>
+        <v>64</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" ref="D13:I13" si="0">MIN(D11,D12)</f>
+        <v>64</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="12">
+        <f>ROUNDUP(C1/C2/C13, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="12">
+        <f>ROUNDUP(D1/D2/D13, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E15" s="12">
+        <f>ROUNDUP(E1/E2/E13, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="F15" s="12">
+        <f>ROUNDUP(F1/F2/F13, 0)</f>
+        <v>16</v>
+      </c>
+      <c r="G15" s="12">
+        <f>ROUNDUP(G1/G2/G13, 0)</f>
+        <v>79</v>
+      </c>
+      <c r="H15" s="12">
+        <f>ROUNDUP(H1/H2/H13, 0)</f>
+        <v>125</v>
+      </c>
+      <c r="I15" s="13">
+        <f>ROUNDUP(I1/I2/I13, 0)</f>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="15">
+        <f>C9*C15</f>
+        <v>0.95</v>
+      </c>
+      <c r="D16" s="15">
+        <f t="shared" ref="D16:I16" si="1">D9*D15</f>
+        <v>0.95</v>
+      </c>
+      <c r="E16" s="15">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="F16" s="15">
+        <f t="shared" si="1"/>
+        <v>15.2</v>
+      </c>
+      <c r="G16" s="15">
+        <f t="shared" si="1"/>
+        <v>75.05</v>
+      </c>
+      <c r="H16" s="15">
+        <f t="shared" si="1"/>
+        <v>118.75</v>
+      </c>
+      <c r="I16" s="16">
+        <f t="shared" si="1"/>
+        <v>149.15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K17" s="9"/>
+    </row>
+    <row r="20" spans="2:11" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B20:I20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
add currency of price
</commit_message>
<xml_diff>
--- a/utils/pricing_estimate.xlsx
+++ b/utils/pricing_estimate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prbejgum\Documents\azure\practice\glasswall_solutions\p-k8-jmeter-test-engine-v1\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1834ED6A-E661-4F96-A5C5-80946FD288E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D41EA32-03A8-4F9C-B0E6-73B6476CEB3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4960AB14-B5A5-4162-B250-4B87383966BE}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     </r>
   </si>
   <si>
-    <t>Total nodes price/hr</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -155,6 +152,9 @@
       <t xml:space="preserve"> This sheet calculates the pricing with varying number of requests for a given node size and fixed pod resources requirement.
 Use sheet1 to decide which node size is best to reduce the overall price and resource wastage.</t>
     </r>
+  </si>
+  <si>
+    <t>Total price/hr in USD</t>
   </si>
 </sst>
 </file>
@@ -186,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -194,110 +194,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +527,7 @@
   <dimension ref="B1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,7 +760,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <f>C10*C16</f>
@@ -868,22 +780,22 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:6" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="B22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -900,7 +812,7 @@
   <dimension ref="B1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:I20"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,422 +823,422 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6">
+      <c r="C1" s="8">
         <v>10</v>
       </c>
-      <c r="D1" s="6">
+      <c r="D1" s="8">
         <v>1000</v>
       </c>
-      <c r="E1" s="6">
+      <c r="E1" s="8">
         <v>10000</v>
       </c>
-      <c r="F1" s="6">
+      <c r="F1" s="8">
         <v>100000</v>
       </c>
-      <c r="G1" s="6">
+      <c r="G1" s="8">
         <v>500000</v>
       </c>
-      <c r="H1" s="6">
+      <c r="H1" s="8">
         <v>800000</v>
       </c>
-      <c r="I1" s="7">
+      <c r="I1" s="8">
         <v>1000000</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="4">
         <v>100</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="4">
         <v>100</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="4">
         <v>100</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="4">
         <v>100</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="4">
         <v>100</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="4">
         <v>100</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="4">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="4">
         <v>250</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="4">
         <v>250</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="4">
         <v>250</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="4">
         <v>250</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="4">
         <v>250</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="4">
         <v>250</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="4">
         <v>250</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9">
-        <v>500</v>
-      </c>
-      <c r="D4" s="9">
-        <v>500</v>
-      </c>
-      <c r="E4" s="9">
-        <v>500</v>
-      </c>
-      <c r="F4" s="9">
-        <v>500</v>
-      </c>
-      <c r="G4" s="9">
-        <v>500</v>
-      </c>
-      <c r="H4" s="9">
-        <v>500</v>
-      </c>
-      <c r="I4" s="10">
+      <c r="C4" s="4">
+        <v>500</v>
+      </c>
+      <c r="D4" s="4">
+        <v>500</v>
+      </c>
+      <c r="E4" s="4">
+        <v>500</v>
+      </c>
+      <c r="F4" s="4">
+        <v>500</v>
+      </c>
+      <c r="G4" s="4">
+        <v>500</v>
+      </c>
+      <c r="H4" s="4">
+        <v>500</v>
+      </c>
+      <c r="I4" s="4">
         <v>500</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="4">
         <v>16</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="4">
         <v>16</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="4">
         <v>16</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="4">
         <v>16</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="4">
         <v>16</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="4">
         <v>16</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="4">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="4">
         <v>32</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="4">
         <v>32</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="4">
         <v>32</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="4">
         <v>32</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="4">
         <v>32</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="4">
         <v>32</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="4">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="4">
         <v>0.95</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="4">
         <v>0.95</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="4">
         <v>0.95</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="4">
         <v>0.95</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="4">
         <v>0.95</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="4">
         <v>0.95</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="4">
         <v>0.95</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="9">
-        <f>C7*1000/C3</f>
-        <v>64</v>
-      </c>
-      <c r="D11" s="9">
-        <f>D7*1000/D3</f>
-        <v>64</v>
-      </c>
-      <c r="E11" s="9">
-        <f>E7*1000/E3</f>
-        <v>64</v>
-      </c>
-      <c r="F11" s="9">
-        <f>F7*1000/F3</f>
-        <v>64</v>
-      </c>
-      <c r="G11" s="9">
-        <f>G7*1000/G3</f>
-        <v>64</v>
-      </c>
-      <c r="H11" s="9">
-        <f>H7*1000/H3</f>
-        <v>64</v>
-      </c>
-      <c r="I11" s="10">
-        <f>I7*1000/I3</f>
+      <c r="C11" s="4">
+        <f t="shared" ref="C11:I11" si="0">C7*1000/C3</f>
+        <v>64</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="9">
-        <f>ROUNDDOWN(C8*1024/C4,0)</f>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12:I12" si="1">ROUNDDOWN(C8*1024/C4,0)</f>
         <v>65</v>
       </c>
-      <c r="D12" s="9">
-        <f>ROUNDDOWN(D8*1024/D4,0)</f>
+      <c r="D12" s="4">
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="E12" s="9">
-        <f>ROUNDDOWN(E8*1024/E4,0)</f>
+      <c r="E12" s="4">
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="F12" s="9">
-        <f>ROUNDDOWN(F8*1024/F4,0)</f>
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="G12" s="9">
-        <f>ROUNDDOWN(G8*1024/G4,0)</f>
+      <c r="G12" s="4">
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="H12" s="9">
-        <f>ROUNDDOWN(H8*1024/H4,0)</f>
+      <c r="H12" s="4">
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="I12" s="10">
-        <f>ROUNDDOWN(I8*1024/I4,0)</f>
+      <c r="I12" s="4">
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="4">
         <f>MIN(C11,C12)</f>
         <v>64</v>
       </c>
-      <c r="D13" s="9">
-        <f t="shared" ref="D13:I13" si="0">MIN(D11,D12)</f>
-        <v>64</v>
-      </c>
-      <c r="E13" s="9">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="F13" s="9">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="G13" s="9">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="I13" s="10">
-        <f t="shared" si="0"/>
+      <c r="D13" s="4">
+        <f t="shared" ref="D13:I13" si="2">MIN(D11,D12)</f>
+        <v>64</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="12">
-        <f>ROUNDUP(C1/C2/C13, 0)</f>
+      <c r="C15" s="5">
+        <f t="shared" ref="C15:I15" si="3">ROUNDUP(C1/C2/C13, 0)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="12">
-        <f>ROUNDUP(D1/D2/D13, 0)</f>
+      <c r="D15" s="5">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="E15" s="12">
-        <f>ROUNDUP(E1/E2/E13, 0)</f>
+      <c r="E15" s="5">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="F15" s="12">
-        <f>ROUNDUP(F1/F2/F13, 0)</f>
+      <c r="F15" s="5">
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="G15" s="12">
-        <f>ROUNDUP(G1/G2/G13, 0)</f>
+      <c r="G15" s="5">
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
-      <c r="H15" s="12">
-        <f>ROUNDUP(H1/H2/H13, 0)</f>
+      <c r="H15" s="5">
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
-      <c r="I15" s="13">
-        <f>ROUNDUP(I1/I2/I13, 0)</f>
+      <c r="I15" s="5">
+        <f t="shared" si="3"/>
         <v>157</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="15">
+      <c r="B16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="4">
         <f>C9*C15</f>
         <v>0.95</v>
       </c>
-      <c r="D16" s="15">
-        <f t="shared" ref="D16:I16" si="1">D9*D15</f>
+      <c r="D16" s="4">
+        <f t="shared" ref="D16:I16" si="4">D9*D15</f>
         <v>0.95</v>
       </c>
-      <c r="E16" s="15">
-        <f t="shared" si="1"/>
+      <c r="E16" s="4">
+        <f t="shared" si="4"/>
         <v>1.9</v>
       </c>
-      <c r="F16" s="15">
-        <f t="shared" si="1"/>
+      <c r="F16" s="4">
+        <f t="shared" si="4"/>
         <v>15.2</v>
       </c>
-      <c r="G16" s="15">
-        <f t="shared" si="1"/>
+      <c r="G16" s="4">
+        <f t="shared" si="4"/>
         <v>75.05</v>
       </c>
-      <c r="H16" s="15">
-        <f t="shared" si="1"/>
+      <c r="H16" s="4">
+        <f t="shared" si="4"/>
         <v>118.75</v>
       </c>
-      <c r="I16" s="16">
-        <f t="shared" si="1"/>
+      <c r="I16" s="4">
+        <f t="shared" si="4"/>
         <v>149.15</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K17" s="9"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="20" spans="2:11" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="B20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>